<commit_message>
Putting together results table
</commit_message>
<xml_diff>
--- a/Results/Simulation5/All_results.xlsx
+++ b/Results/Simulation5/All_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Unsampled</t>
   </si>
@@ -88,6 +88,42 @@
   </si>
   <si>
     <t>10 Median</t>
+  </si>
+  <si>
+    <t>specificity.25.</t>
+  </si>
+  <si>
+    <t>sensitivity.25.</t>
+  </si>
+  <si>
+    <t>accuracy.25.</t>
+  </si>
+  <si>
+    <t>threshold.25.</t>
+  </si>
+  <si>
+    <t>AUC.25.</t>
+  </si>
+  <si>
+    <t>specificity.75.</t>
+  </si>
+  <si>
+    <t>sensitivity.75.</t>
+  </si>
+  <si>
+    <t>accuracy.75.</t>
+  </si>
+  <si>
+    <t>threshold.75.</t>
+  </si>
+  <si>
+    <t>AUC.75.</t>
+  </si>
+  <si>
+    <t>25 Quantile</t>
+  </si>
+  <si>
+    <t>75 Quantile</t>
   </si>
 </sst>
 </file>
@@ -489,15 +525,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -540,8 +576,44 @@
       <c r="N1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -581,8 +653,38 @@
       <c r="N2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>97</v>
+      </c>
+      <c r="S2">
+        <v>50</v>
+      </c>
+      <c r="T2">
+        <v>78</v>
+      </c>
+      <c r="V2">
+        <v>100</v>
+      </c>
+      <c r="W2">
+        <v>3</v>
+      </c>
+      <c r="X2">
+        <v>97</v>
+      </c>
+      <c r="Y2">
+        <v>50</v>
+      </c>
+      <c r="Z2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -622,8 +724,38 @@
       <c r="N3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="P3">
+        <v>72</v>
+      </c>
+      <c r="Q3">
+        <v>67</v>
+      </c>
+      <c r="R3">
+        <v>72</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>78</v>
+      </c>
+      <c r="V3">
+        <v>78</v>
+      </c>
+      <c r="W3">
+        <v>74</v>
+      </c>
+      <c r="X3">
+        <v>78</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -663,8 +795,38 @@
       <c r="N4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P4">
+        <v>71</v>
+      </c>
+      <c r="Q4">
+        <v>66</v>
+      </c>
+      <c r="R4">
+        <v>71</v>
+      </c>
+      <c r="S4">
+        <v>46</v>
+      </c>
+      <c r="T4">
+        <v>77</v>
+      </c>
+      <c r="V4">
+        <v>78</v>
+      </c>
+      <c r="W4">
+        <v>74</v>
+      </c>
+      <c r="X4">
+        <v>78</v>
+      </c>
+      <c r="Y4">
+        <v>52</v>
+      </c>
+      <c r="Z4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -704,8 +866,38 @@
       <c r="N5">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="P5">
+        <v>71</v>
+      </c>
+      <c r="Q5">
+        <v>66</v>
+      </c>
+      <c r="R5">
+        <v>71</v>
+      </c>
+      <c r="S5">
+        <v>45</v>
+      </c>
+      <c r="T5">
+        <v>77</v>
+      </c>
+      <c r="V5">
+        <v>78</v>
+      </c>
+      <c r="W5">
+        <v>74</v>
+      </c>
+      <c r="X5">
+        <v>78</v>
+      </c>
+      <c r="Y5">
+        <v>52</v>
+      </c>
+      <c r="Z5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -745,8 +937,38 @@
       <c r="N6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="P6">
+        <v>71</v>
+      </c>
+      <c r="Q6">
+        <v>66</v>
+      </c>
+      <c r="R6">
+        <v>71</v>
+      </c>
+      <c r="S6">
+        <v>38</v>
+      </c>
+      <c r="T6">
+        <v>77</v>
+      </c>
+      <c r="V6">
+        <v>78</v>
+      </c>
+      <c r="W6">
+        <v>73</v>
+      </c>
+      <c r="X6">
+        <v>77</v>
+      </c>
+      <c r="Y6">
+        <v>44</v>
+      </c>
+      <c r="Z6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -754,7 +976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -794,8 +1016,38 @@
       <c r="N8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>95</v>
+      </c>
+      <c r="S8">
+        <v>50</v>
+      </c>
+      <c r="T8">
+        <v>78</v>
+      </c>
+      <c r="V8">
+        <v>100</v>
+      </c>
+      <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <v>95</v>
+      </c>
+      <c r="Y8">
+        <v>50</v>
+      </c>
+      <c r="Z8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -835,8 +1087,38 @@
       <c r="N9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="P9">
+        <v>72</v>
+      </c>
+      <c r="Q9">
+        <v>67</v>
+      </c>
+      <c r="R9">
+        <v>72</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <v>78</v>
+      </c>
+      <c r="V9">
+        <v>77</v>
+      </c>
+      <c r="W9">
+        <v>72</v>
+      </c>
+      <c r="X9">
+        <v>76</v>
+      </c>
+      <c r="Y9">
+        <v>6</v>
+      </c>
+      <c r="Z9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -876,8 +1158,38 @@
       <c r="N10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="P10">
+        <v>71</v>
+      </c>
+      <c r="Q10">
+        <v>66</v>
+      </c>
+      <c r="R10">
+        <v>72</v>
+      </c>
+      <c r="S10">
+        <v>46</v>
+      </c>
+      <c r="T10">
+        <v>77</v>
+      </c>
+      <c r="V10">
+        <v>77</v>
+      </c>
+      <c r="W10">
+        <v>72</v>
+      </c>
+      <c r="X10">
+        <v>76</v>
+      </c>
+      <c r="Y10">
+        <v>51</v>
+      </c>
+      <c r="Z10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -917,8 +1229,38 @@
       <c r="N11">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="P11">
+        <v>71</v>
+      </c>
+      <c r="Q11">
+        <v>67</v>
+      </c>
+      <c r="R11">
+        <v>71</v>
+      </c>
+      <c r="S11">
+        <v>46</v>
+      </c>
+      <c r="T11">
+        <v>77</v>
+      </c>
+      <c r="V11">
+        <v>77</v>
+      </c>
+      <c r="W11">
+        <v>72</v>
+      </c>
+      <c r="X11">
+        <v>76</v>
+      </c>
+      <c r="Y11">
+        <v>51</v>
+      </c>
+      <c r="Z11">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -958,8 +1300,38 @@
       <c r="N12">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="P12">
+        <v>71</v>
+      </c>
+      <c r="Q12">
+        <v>66</v>
+      </c>
+      <c r="R12">
+        <v>71</v>
+      </c>
+      <c r="S12">
+        <v>39</v>
+      </c>
+      <c r="T12">
+        <v>77</v>
+      </c>
+      <c r="V12">
+        <v>77</v>
+      </c>
+      <c r="W12">
+        <v>72</v>
+      </c>
+      <c r="X12">
+        <v>76</v>
+      </c>
+      <c r="Y12">
+        <v>44</v>
+      </c>
+      <c r="Z12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -967,7 +1339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1007,8 +1379,38 @@
       <c r="N14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="P14">
+        <v>99</v>
+      </c>
+      <c r="Q14">
+        <v>7</v>
+      </c>
+      <c r="R14">
+        <v>90</v>
+      </c>
+      <c r="S14">
+        <v>50</v>
+      </c>
+      <c r="T14">
+        <v>77</v>
+      </c>
+      <c r="V14">
+        <v>100</v>
+      </c>
+      <c r="W14">
+        <v>9</v>
+      </c>
+      <c r="X14">
+        <v>91</v>
+      </c>
+      <c r="Y14">
+        <v>50</v>
+      </c>
+      <c r="Z14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1048,8 +1450,38 @@
       <c r="N15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="P15">
+        <v>72</v>
+      </c>
+      <c r="Q15">
+        <v>66</v>
+      </c>
+      <c r="R15">
+        <v>71</v>
+      </c>
+      <c r="S15">
+        <v>9</v>
+      </c>
+      <c r="T15">
+        <v>77</v>
+      </c>
+      <c r="V15">
+        <v>76</v>
+      </c>
+      <c r="W15">
+        <v>70</v>
+      </c>
+      <c r="X15">
+        <v>75</v>
+      </c>
+      <c r="Y15">
+        <v>11</v>
+      </c>
+      <c r="Z15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1089,8 +1521,38 @@
       <c r="N16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="P16">
+        <v>71</v>
+      </c>
+      <c r="Q16">
+        <v>66</v>
+      </c>
+      <c r="R16">
+        <v>71</v>
+      </c>
+      <c r="S16">
+        <v>47</v>
+      </c>
+      <c r="T16">
+        <v>77</v>
+      </c>
+      <c r="V16">
+        <v>76</v>
+      </c>
+      <c r="W16">
+        <v>71</v>
+      </c>
+      <c r="X16">
+        <v>75</v>
+      </c>
+      <c r="Y16">
+        <v>51</v>
+      </c>
+      <c r="Z16">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1130,8 +1592,38 @@
       <c r="N17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="P17">
+        <v>71</v>
+      </c>
+      <c r="Q17">
+        <v>66</v>
+      </c>
+      <c r="R17">
+        <v>71</v>
+      </c>
+      <c r="S17">
+        <v>47</v>
+      </c>
+      <c r="T17">
+        <v>77</v>
+      </c>
+      <c r="V17">
+        <v>76</v>
+      </c>
+      <c r="W17">
+        <v>70</v>
+      </c>
+      <c r="X17">
+        <v>75</v>
+      </c>
+      <c r="Y17">
+        <v>51</v>
+      </c>
+      <c r="Z17">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1171,8 +1663,38 @@
       <c r="N18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="P18">
+        <v>71</v>
+      </c>
+      <c r="Q18">
+        <v>66</v>
+      </c>
+      <c r="R18">
+        <v>71</v>
+      </c>
+      <c r="S18">
+        <v>39</v>
+      </c>
+      <c r="T18">
+        <v>76</v>
+      </c>
+      <c r="V18">
+        <v>75</v>
+      </c>
+      <c r="W18">
+        <v>70</v>
+      </c>
+      <c r="X18">
+        <v>74</v>
+      </c>
+      <c r="Y18">
+        <v>44</v>
+      </c>
+      <c r="Z18">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:26">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1220,8 +1742,38 @@
       <c r="N20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="P20">
+        <v>97</v>
+      </c>
+      <c r="Q20">
+        <v>21</v>
+      </c>
+      <c r="R20">
+        <v>82</v>
+      </c>
+      <c r="S20">
+        <v>50</v>
+      </c>
+      <c r="T20">
+        <v>76</v>
+      </c>
+      <c r="V20">
+        <v>97</v>
+      </c>
+      <c r="W20">
+        <v>22</v>
+      </c>
+      <c r="X20">
+        <v>83</v>
+      </c>
+      <c r="Y20">
+        <v>50</v>
+      </c>
+      <c r="Z20">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1261,8 +1813,38 @@
       <c r="N21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="P21">
+        <v>71</v>
+      </c>
+      <c r="Q21">
+        <v>63</v>
+      </c>
+      <c r="R21">
+        <v>70</v>
+      </c>
+      <c r="S21">
+        <v>19</v>
+      </c>
+      <c r="T21">
+        <v>76</v>
+      </c>
+      <c r="V21">
+        <v>76</v>
+      </c>
+      <c r="W21">
+        <v>68</v>
+      </c>
+      <c r="X21">
+        <v>74</v>
+      </c>
+      <c r="Y21">
+        <v>21</v>
+      </c>
+      <c r="Z21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1302,8 +1884,38 @@
       <c r="N22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="P22">
+        <v>70</v>
+      </c>
+      <c r="Q22">
+        <v>63</v>
+      </c>
+      <c r="R22">
+        <v>70</v>
+      </c>
+      <c r="S22">
+        <v>47</v>
+      </c>
+      <c r="T22">
+        <v>75</v>
+      </c>
+      <c r="V22">
+        <v>76</v>
+      </c>
+      <c r="W22">
+        <v>69</v>
+      </c>
+      <c r="X22">
+        <v>73</v>
+      </c>
+      <c r="Y22">
+        <v>51</v>
+      </c>
+      <c r="Z22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1343,8 +1955,38 @@
       <c r="N23">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="P23">
+        <v>71</v>
+      </c>
+      <c r="Q23">
+        <v>63</v>
+      </c>
+      <c r="R23">
+        <v>70</v>
+      </c>
+      <c r="S23">
+        <v>47</v>
+      </c>
+      <c r="T23">
+        <v>75</v>
+      </c>
+      <c r="V23">
+        <v>76</v>
+      </c>
+      <c r="W23">
+        <v>68</v>
+      </c>
+      <c r="X23">
+        <v>73</v>
+      </c>
+      <c r="Y23">
+        <v>51</v>
+      </c>
+      <c r="Z23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1384,8 +2026,38 @@
       <c r="N24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="P24">
+        <v>71</v>
+      </c>
+      <c r="Q24">
+        <v>64</v>
+      </c>
+      <c r="R24">
+        <v>70</v>
+      </c>
+      <c r="S24">
+        <v>40</v>
+      </c>
+      <c r="T24">
+        <v>75</v>
+      </c>
+      <c r="V24">
+        <v>75</v>
+      </c>
+      <c r="W24">
+        <v>68</v>
+      </c>
+      <c r="X24">
+        <v>73</v>
+      </c>
+      <c r="Y24">
+        <v>44</v>
+      </c>
+      <c r="Z24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1393,7 +2065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:26">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1433,8 +2105,38 @@
       <c r="N26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="P26">
+        <v>84</v>
+      </c>
+      <c r="Q26">
+        <v>48</v>
+      </c>
+      <c r="R26">
+        <v>70</v>
+      </c>
+      <c r="S26">
+        <v>50</v>
+      </c>
+      <c r="T26">
+        <v>74</v>
+      </c>
+      <c r="V26">
+        <v>85</v>
+      </c>
+      <c r="W26">
+        <v>49</v>
+      </c>
+      <c r="X26">
+        <v>70</v>
+      </c>
+      <c r="Y26">
+        <v>50</v>
+      </c>
+      <c r="Z26">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1474,8 +2176,38 @@
       <c r="N27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="P27">
+        <v>69</v>
+      </c>
+      <c r="Q27">
+        <v>64</v>
+      </c>
+      <c r="R27">
+        <v>68</v>
+      </c>
+      <c r="S27">
+        <v>38</v>
+      </c>
+      <c r="T27">
+        <v>74</v>
+      </c>
+      <c r="V27">
+        <v>72</v>
+      </c>
+      <c r="W27">
+        <v>67</v>
+      </c>
+      <c r="X27">
+        <v>69</v>
+      </c>
+      <c r="Y27">
+        <v>41</v>
+      </c>
+      <c r="Z27">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1515,8 +2247,38 @@
       <c r="N28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="P28">
+        <v>69</v>
+      </c>
+      <c r="Q28">
+        <v>64</v>
+      </c>
+      <c r="R28">
+        <v>68</v>
+      </c>
+      <c r="S28">
+        <v>47</v>
+      </c>
+      <c r="T28">
+        <v>74</v>
+      </c>
+      <c r="V28">
+        <v>72</v>
+      </c>
+      <c r="W28">
+        <v>67</v>
+      </c>
+      <c r="X28">
+        <v>69</v>
+      </c>
+      <c r="Y28">
+        <v>50</v>
+      </c>
+      <c r="Z28">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1556,8 +2318,38 @@
       <c r="N29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="P29">
+        <v>69</v>
+      </c>
+      <c r="Q29">
+        <v>64</v>
+      </c>
+      <c r="R29">
+        <v>68</v>
+      </c>
+      <c r="S29">
+        <v>47</v>
+      </c>
+      <c r="T29">
+        <v>74</v>
+      </c>
+      <c r="V29">
+        <v>72</v>
+      </c>
+      <c r="W29">
+        <v>67</v>
+      </c>
+      <c r="X29">
+        <v>69</v>
+      </c>
+      <c r="Y29">
+        <v>50</v>
+      </c>
+      <c r="Z29">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1597,8 +2389,38 @@
       <c r="N30">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="P30">
+        <v>68</v>
+      </c>
+      <c r="Q30">
+        <v>62</v>
+      </c>
+      <c r="R30">
+        <v>68</v>
+      </c>
+      <c r="S30">
+        <v>40</v>
+      </c>
+      <c r="T30">
+        <v>73</v>
+      </c>
+      <c r="V30">
+        <v>73</v>
+      </c>
+      <c r="W30">
+        <v>67</v>
+      </c>
+      <c r="X30">
+        <v>69</v>
+      </c>
+      <c r="Y30">
+        <v>43</v>
+      </c>
+      <c r="Z30">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1606,7 +2428,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:26">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1646,8 +2468,38 @@
       <c r="N32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="P32">
+        <v>72</v>
+      </c>
+      <c r="Q32">
+        <v>62</v>
+      </c>
+      <c r="R32">
+        <v>67</v>
+      </c>
+      <c r="S32">
+        <v>50</v>
+      </c>
+      <c r="T32">
+        <v>73</v>
+      </c>
+      <c r="V32">
+        <v>73</v>
+      </c>
+      <c r="W32">
+        <v>63</v>
+      </c>
+      <c r="X32">
+        <v>68</v>
+      </c>
+      <c r="Y32">
+        <v>50</v>
+      </c>
+      <c r="Z32">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1686,6 +2538,36 @@
       </c>
       <c r="N33">
         <v>8</v>
+      </c>
+      <c r="P33">
+        <v>71</v>
+      </c>
+      <c r="Q33">
+        <v>62</v>
+      </c>
+      <c r="R33">
+        <v>67</v>
+      </c>
+      <c r="S33">
+        <v>48</v>
+      </c>
+      <c r="T33">
+        <v>73</v>
+      </c>
+      <c r="V33">
+        <v>73</v>
+      </c>
+      <c r="W33">
+        <v>65</v>
+      </c>
+      <c r="X33">
+        <v>68</v>
+      </c>
+      <c r="Y33">
+        <v>51</v>
+      </c>
+      <c r="Z33">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished sim results tables
One for paper and one for appendix with median and IQR
</commit_message>
<xml_diff>
--- a/Results/Simulation5/All_results.xlsx
+++ b/Results/Simulation5/All_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="0" windowWidth="21440" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="0" windowWidth="21440" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Unsampled</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>75 Quantile</t>
+  </si>
+  <si>
+    <t>*note for quaniltes specificity is first</t>
   </si>
 </sst>
 </file>
@@ -163,12 +166,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFCA2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,22 +189,140 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,7 +740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -652,6 +779,9 @@
       </c>
       <c r="N2">
         <v>6</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="P2">
         <v>100</v>
@@ -724,6 +854,7 @@
       <c r="N3">
         <v>6</v>
       </c>
+      <c r="O3" s="3"/>
       <c r="P3">
         <v>72</v>
       </c>
@@ -795,6 +926,7 @@
       <c r="N4">
         <v>9</v>
       </c>
+      <c r="O4" s="3"/>
       <c r="P4">
         <v>71</v>
       </c>
@@ -866,6 +998,7 @@
       <c r="N5">
         <v>27</v>
       </c>
+      <c r="O5" s="3"/>
       <c r="P5">
         <v>71</v>
       </c>
@@ -937,6 +1070,7 @@
       <c r="N6">
         <v>14</v>
       </c>
+      <c r="O6" s="2"/>
       <c r="P6">
         <v>71</v>
       </c>
@@ -975,6 +1109,7 @@
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
@@ -2571,6 +2706,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O2:O5"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>